<commit_message>
Converted the validity to 75%. Made all non-debug condition rely on a single conditions file. Implemented self-paced trial progression. Implemented condition-specific instructions.
</commit_message>
<xml_diff>
--- a/cond-files/cond_eb1_d.xlsx
+++ b/cond-files/cond_eb1_d.xlsx
@@ -1,49 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\eb\eb\cond-files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F2F69A-10A9-4CA1-B00F-EE4C3117F97A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="150" windowWidth="16260" windowHeight="5595"/>
+    <workbookView xWindow="92" yWindow="144" windowWidth="16259" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_eb1_c" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>targ_right</t>
   </si>
   <si>
     <t>cue_valid</t>
   </si>
-  <si>
-    <t>corr_resp</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>session_id</t>
-  </si>
-  <si>
-    <t>trial_id</t>
-  </si>
-  <si>
-    <t>TRIAL_START</t>
-  </si>
-  <si>
-    <t>TRIAL_END</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,6 +563,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -622,7 +613,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -655,9 +646,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,6 +698,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -865,146 +890,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2">
-        <v>-1</v>
-      </c>
-      <c r="C2">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D2">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-      <c r="H2">
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-1</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D4">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E4">
+      <c r="B5">
         <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>-1</v>
-      </c>
-      <c r="H4">
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-1</v>
-      </c>
-      <c r="B5">
-        <v>-1</v>
-      </c>
-      <c r="C5">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D5">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>-1.1000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>